<commit_message>
Update Projeto integrador e Criação de Arquivos SQL
</commit_message>
<xml_diff>
--- a/Projeto_Integrador/Dashboard Simples com EXCEL/Preços da Gasolina.xlsx
+++ b/Projeto_Integrador/Dashboard Simples com EXCEL/Preços da Gasolina.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84284528572\OneDrive\Documentos\GitHub\Segundo_Semestre_Ciencia_de_Dados\Projeto_Integrador\Dashboard Simples com EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{ED2FA35A-44DB-402F-B4D9-E7785E44643F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{73F6CB95-9CD0-405F-A63E-3EB8E5DE8EDE}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{ED2FA35A-44DB-402F-B4D9-E7785E44643F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{FE43CF3F-E718-4D08-AB50-34D0A60F5F29}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{FC2E7B8D-23B3-4077-9A58-ADB76B526F74}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="20">
   <si>
     <t>ESTADO</t>
   </si>
@@ -80,12 +80,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>PREÇO MÁXIMO</t>
-  </si>
-  <si>
-    <t>PREÇO MÍNIMO</t>
-  </si>
-  <si>
     <t>QUANTIDADE LTS</t>
   </si>
   <si>
@@ -96,6 +90,12 @@
   </si>
   <si>
     <t>DIESEL COMUM</t>
+  </si>
+  <si>
+    <t>PREÇO UNITARIO</t>
+  </si>
+  <si>
+    <t>PREÇO FINAL</t>
   </si>
 </sst>
 </file>
@@ -201,8 +201,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B91DE08B-AF80-4952-898C-64674B4DD81F}" name="gasolina_2010" displayName="gasolina_2010" ref="A1:G61" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G61" xr:uid="{A1934503-5C81-4CC0-A35A-98B943F9F0ED}"/>
-  <sortState ref="A2:G61">
-    <sortCondition ref="C1:C61"/>
+  <sortState ref="A2:G60">
+    <sortCondition ref="C1:C60"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3DA4F2EB-227C-462F-938F-58462056C656}" uniqueName="1" name="ID" queryTableFieldId="1"/>
@@ -210,8 +210,8 @@
     <tableColumn id="5" xr3:uid="{6046F7C5-86BD-4E06-97EF-C223471E2DD2}" uniqueName="5" name="ESTADO" queryTableFieldId="5"/>
     <tableColumn id="6" xr3:uid="{A72EE60D-49E0-4621-9BD9-056D0CEBD585}" uniqueName="6" name="PRODUTO" queryTableFieldId="6"/>
     <tableColumn id="9" xr3:uid="{B48C3883-135E-456D-B0C3-B6B0E8760B09}" uniqueName="9" name="QUANTIDADE LTS" queryTableFieldId="9" dataDxfId="0" dataCellStyle="Moeda"/>
-    <tableColumn id="11" xr3:uid="{7AA556D9-55B1-419F-8393-FF79D880E6BE}" uniqueName="11" name="PREÇO MÍNIMO" queryTableFieldId="11" dataCellStyle="Moeda"/>
-    <tableColumn id="12" xr3:uid="{0A5646F3-54C5-4651-B442-562FF61E1239}" uniqueName="12" name="PREÇO MÁXIMO" queryTableFieldId="12" dataCellStyle="Moeda"/>
+    <tableColumn id="11" xr3:uid="{7AA556D9-55B1-419F-8393-FF79D880E6BE}" uniqueName="11" name="PREÇO UNITARIO" queryTableFieldId="11" dataCellStyle="Moeda"/>
+    <tableColumn id="12" xr3:uid="{0A5646F3-54C5-4651-B442-562FF61E1239}" uniqueName="12" name="PREÇO FINAL" queryTableFieldId="12" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -517,7 +517,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:C44"/>
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,18 +543,18 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>119962</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -572,12 +572,13 @@
         <v>2.98</v>
       </c>
       <c r="G2" s="1">
-        <v>5.59</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>23.84</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>120319</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -586,7 +587,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2">
         <v>6</v>
@@ -595,12 +596,13 @@
         <v>3.266</v>
       </c>
       <c r="G3" s="1">
-        <v>5.7919999999999998</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>19.596</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>119606</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -618,12 +620,13 @@
         <v>3.49</v>
       </c>
       <c r="G4" s="1">
-        <v>5.96</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>27.92</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>119633</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -641,12 +644,13 @@
         <v>3.4260000000000002</v>
       </c>
       <c r="G5" s="1">
-        <v>5.9119999999999999</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>13.704000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>119608</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -655,7 +659,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="2">
         <v>8</v>
@@ -664,12 +668,13 @@
         <v>3.17</v>
       </c>
       <c r="G6" s="1">
-        <v>5.72</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>25.36</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>119786</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -678,7 +683,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2">
         <v>6</v>
@@ -687,12 +692,13 @@
         <v>3.4580000000000002</v>
       </c>
       <c r="G7" s="1">
-        <v>5.9359999999999999</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>20.748000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>120142</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -701,7 +707,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8" s="2">
         <v>4</v>
@@ -710,12 +716,13 @@
         <v>3.746</v>
       </c>
       <c r="G8" s="1">
-        <v>6.1520000000000001</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>14.984</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>120678</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -724,7 +731,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E9" s="2">
         <v>6</v>
@@ -733,12 +740,13 @@
         <v>3.778</v>
       </c>
       <c r="G9" s="1">
-        <v>6.1760000000000002</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>22.667999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>120679</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -747,7 +755,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E10" s="2">
         <v>4</v>
@@ -756,12 +764,13 @@
         <v>3.234</v>
       </c>
       <c r="G10" s="1">
-        <v>5.7679999999999998</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>12.936</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>119610</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -779,12 +788,13 @@
         <v>3.5219999999999998</v>
       </c>
       <c r="G11" s="1">
-        <v>5.984</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>35.22</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>119788</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
@@ -802,12 +812,13 @@
         <v>3.6179999999999999</v>
       </c>
       <c r="G12" s="1">
-        <v>6.056</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>21.707999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>119430</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -825,12 +836,13 @@
         <v>3.65</v>
       </c>
       <c r="G13" s="1">
-        <v>6.08</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>29.2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>119966</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -839,7 +851,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E14" s="2">
         <v>10</v>
@@ -848,12 +860,13 @@
         <v>3.6819999999999999</v>
       </c>
       <c r="G14" s="1">
-        <v>6.1040000000000001</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>36.82</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>119613</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -871,12 +884,13 @@
         <v>3.5859999999999999</v>
       </c>
       <c r="G15" s="1">
-        <v>6.032</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>14.343999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>118722</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -885,7 +899,7 @@
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E16" s="2">
         <v>8</v>
@@ -894,12 +908,13 @@
         <v>3.1379999999999999</v>
       </c>
       <c r="G16" s="1">
-        <v>5.6959999999999997</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>25.103999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>120148</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -908,7 +923,7 @@
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E17" s="2">
         <v>2</v>
@@ -917,12 +932,13 @@
         <v>3.714</v>
       </c>
       <c r="G17" s="1">
-        <v>6.1280000000000001</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>7.4279999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>119434</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -931,7 +947,7 @@
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E18" s="2">
         <v>8</v>
@@ -940,12 +956,13 @@
         <v>3.778</v>
       </c>
       <c r="G18" s="1">
-        <v>6.1760000000000002</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>30.224</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>119619</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -963,12 +980,13 @@
         <v>3.5539999999999998</v>
       </c>
       <c r="G19" s="1">
-        <v>6.008</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>7.1079999999999997</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>119620</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -986,12 +1004,13 @@
         <v>2.95</v>
       </c>
       <c r="G20" s="1">
-        <v>5.52</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>17.700000000000003</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>119440</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -1009,12 +1028,13 @@
         <v>3.01</v>
       </c>
       <c r="G21" s="1">
-        <v>5.6</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>30.099999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>120154</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -1023,7 +1043,7 @@
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E22" s="2">
         <v>8</v>
@@ -1032,12 +1052,13 @@
         <v>3.298</v>
       </c>
       <c r="G22" s="1">
-        <v>5.8159999999999998</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>26.384</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>120690</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -1046,7 +1067,7 @@
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E23" s="2">
         <v>8</v>
@@ -1055,12 +1076,13 @@
         <v>3.4580000000000002</v>
       </c>
       <c r="G23" s="1">
-        <v>5.9359999999999999</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>27.664000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>119976</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -1069,7 +1091,7 @@
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E24" s="2">
         <v>10</v>
@@ -1078,12 +1100,13 @@
         <v>3.49</v>
       </c>
       <c r="G24" s="1">
-        <v>5.96</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>34.900000000000006</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>119260</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -1092,7 +1115,7 @@
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E25" s="2">
         <v>2</v>
@@ -1101,12 +1124,13 @@
         <v>3.5219999999999998</v>
       </c>
       <c r="G25" s="1">
-        <v>5.984</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>7.0439999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>119798</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -1115,7 +1139,7 @@
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E26" s="2">
         <v>4</v>
@@ -1124,12 +1148,13 @@
         <v>3.5539999999999998</v>
       </c>
       <c r="G26" s="1">
-        <v>6.008</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>14.215999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>120511</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
@@ -1138,7 +1163,7 @@
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E27" s="2">
         <v>2</v>
@@ -1147,12 +1172,13 @@
         <v>3.6819999999999999</v>
       </c>
       <c r="G27" s="1">
-        <v>6.1040000000000001</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>7.3639999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>120333</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -1161,7 +1187,7 @@
         <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E28" s="2">
         <v>4</v>
@@ -1170,12 +1196,13 @@
         <v>3.714</v>
       </c>
       <c r="G28" s="1">
-        <v>6.1280000000000001</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>14.856</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>119647</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -1193,12 +1220,13 @@
         <v>3.778</v>
       </c>
       <c r="G29" s="1">
-        <v>6.1760000000000002</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>30.224</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>119825</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -1216,12 +1244,13 @@
         <v>3.01</v>
       </c>
       <c r="G30" s="1">
-        <v>5.6</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>24.08</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>120538</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -1239,12 +1268,13 @@
         <v>3.1379999999999999</v>
       </c>
       <c r="G31" s="1">
-        <v>5.6959999999999997</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>18.827999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>120717</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -1262,12 +1292,13 @@
         <v>3.202</v>
       </c>
       <c r="G32" s="1">
-        <v>5.7439999999999998</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>32.019999999999996</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>120003</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -1285,12 +1316,13 @@
         <v>3.266</v>
       </c>
       <c r="G33" s="1">
-        <v>5.7919999999999998</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>13.064</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>120360</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -1308,12 +1340,13 @@
         <v>3.298</v>
       </c>
       <c r="G34" s="1">
-        <v>5.8159999999999998</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>19.788</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>120181</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -1331,12 +1364,13 @@
         <v>3.33</v>
       </c>
       <c r="G35" s="1">
-        <v>5.84</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>26.64</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>119467</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
@@ -1354,12 +1388,13 @@
         <v>3.3940000000000001</v>
       </c>
       <c r="G36" s="1">
-        <v>5.8879999999999999</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>6.7880000000000003</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>119442</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
@@ -1368,7 +1403,7 @@
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E37" s="2">
         <v>10</v>
@@ -1377,12 +1412,13 @@
         <v>3.33</v>
       </c>
       <c r="G37" s="1">
-        <v>5.84</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>33.299999999999997</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>119622</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
@@ -1391,7 +1427,7 @@
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E38" s="2">
         <v>6</v>
@@ -1400,12 +1436,13 @@
         <v>3.4260000000000002</v>
       </c>
       <c r="G38" s="1">
-        <v>5.9119999999999999</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>20.556000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>120692</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
@@ -1414,7 +1451,7 @@
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E39" s="2">
         <v>6</v>
@@ -1423,12 +1460,13 @@
         <v>3.5859999999999999</v>
       </c>
       <c r="G39" s="1">
-        <v>6.032</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>21.515999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>120156</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
@@ -1437,7 +1475,7 @@
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E40" s="2">
         <v>8</v>
@@ -1446,12 +1484,13 @@
         <v>3.6179999999999999</v>
       </c>
       <c r="G40" s="1">
-        <v>6.056</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>28.943999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>120335</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>6</v>
@@ -1460,7 +1499,7 @@
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E41" s="2">
         <v>10</v>
@@ -1469,12 +1508,13 @@
         <v>3.65</v>
       </c>
       <c r="G41" s="1">
-        <v>6.08</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>36.5</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>120513</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>
@@ -1483,7 +1523,7 @@
         <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E42" s="2">
         <v>6</v>
@@ -1492,12 +1532,13 @@
         <v>2.98</v>
       </c>
       <c r="G42" s="1">
-        <v>5.59</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>17.88</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>119800</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>6</v>
@@ -1506,7 +1547,7 @@
         <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E43" s="2">
         <v>10</v>
@@ -1515,12 +1556,13 @@
         <v>3.3620000000000001</v>
       </c>
       <c r="G43" s="1">
-        <v>5.8639999999999999</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>33.620000000000005</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>119469</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>6</v>
@@ -1538,12 +1580,13 @@
         <v>3.746</v>
       </c>
       <c r="G44" s="1">
-        <v>6.1520000000000001</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>22.475999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>119649</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>6</v>
@@ -1561,12 +1604,13 @@
         <v>2.95</v>
       </c>
       <c r="G45" s="1">
-        <v>5.52</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>11.8</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>120719</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>6</v>
@@ -1584,12 +1628,13 @@
         <v>3.0419999999999998</v>
       </c>
       <c r="G46" s="1">
-        <v>5.6239999999999997</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>30.419999999999998</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>120183</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>6</v>
@@ -1607,12 +1652,13 @@
         <v>3.0739999999999998</v>
       </c>
       <c r="G47" s="1">
-        <v>5.6479999999999997</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>6.1479999999999997</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>120362</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>6</v>
@@ -1630,12 +1676,13 @@
         <v>3.1059999999999999</v>
       </c>
       <c r="G48" s="1">
-        <v>5.6719999999999997</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>12.423999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>120540</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>6</v>
@@ -1653,12 +1700,13 @@
         <v>3.234</v>
       </c>
       <c r="G49" s="1">
-        <v>5.7679999999999998</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>6.468</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>119982</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>6</v>
@@ -1676,12 +1724,13 @@
         <v>2.89</v>
       </c>
       <c r="G50" s="1">
-        <v>5.5</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>5.78</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>119446</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>6</v>
@@ -1699,12 +1748,13 @@
         <v>2.9</v>
       </c>
       <c r="G51" s="1">
-        <v>5.55</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>11.6</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>120696</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>6</v>
@@ -1713,7 +1763,7 @@
         <v>9</v>
       </c>
       <c r="D52" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E52" s="2">
         <v>2</v>
@@ -1722,12 +1772,13 @@
         <v>3.0419999999999998</v>
       </c>
       <c r="G52" s="1">
-        <v>5.6239999999999997</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>6.0839999999999996</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>119626</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>6</v>
@@ -1736,7 +1787,7 @@
         <v>9</v>
       </c>
       <c r="D53" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E53" s="2">
         <v>4</v>
@@ -1745,12 +1796,13 @@
         <v>3.0739999999999998</v>
       </c>
       <c r="G53" s="1">
-        <v>5.6479999999999997</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>12.295999999999999</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>119804</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>6</v>
@@ -1759,7 +1811,7 @@
         <v>9</v>
       </c>
       <c r="D54" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E54" s="2">
         <v>6</v>
@@ -1768,12 +1820,13 @@
         <v>3.1059999999999999</v>
       </c>
       <c r="G54" s="1">
-        <v>5.6719999999999997</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>18.635999999999999</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>120339</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>6</v>
@@ -1782,7 +1835,7 @@
         <v>9</v>
       </c>
       <c r="D55" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E55" s="2">
         <v>10</v>
@@ -1791,12 +1844,13 @@
         <v>3.17</v>
       </c>
       <c r="G55" s="1">
-        <v>5.72</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>31.7</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>120160</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>6</v>
@@ -1805,7 +1859,7 @@
         <v>9</v>
       </c>
       <c r="D56" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E56" s="2">
         <v>2</v>
@@ -1814,12 +1868,13 @@
         <v>3.202</v>
       </c>
       <c r="G56" s="1">
-        <v>5.7439999999999998</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>6.4039999999999999</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>120517</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>6</v>
@@ -1828,7 +1883,7 @@
         <v>9</v>
       </c>
       <c r="D57" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E57" s="2">
         <v>2</v>
@@ -1837,12 +1892,13 @@
         <v>3.3620000000000001</v>
       </c>
       <c r="G57" s="1">
-        <v>5.8639999999999999</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>6.7240000000000002</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>119089</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
@@ -1851,7 +1907,7 @@
         <v>9</v>
       </c>
       <c r="D58" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E58" s="2">
         <v>4</v>
@@ -1860,12 +1916,13 @@
         <v>3.3940000000000001</v>
       </c>
       <c r="G58" s="1">
-        <v>5.8879999999999999</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>13.576000000000001</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>119266</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>6</v>
@@ -1874,7 +1931,7 @@
         <v>9</v>
       </c>
       <c r="D59" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E59" s="2">
         <v>10</v>
@@ -1883,12 +1940,13 @@
         <v>2.89</v>
       </c>
       <c r="G59" s="1">
-        <v>5.5</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>28.900000000000002</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>118911</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>6</v>
@@ -1897,7 +1955,7 @@
         <v>9</v>
       </c>
       <c r="D60" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E60" s="2">
         <v>2</v>
@@ -1906,11 +1964,33 @@
         <v>2.9</v>
       </c>
       <c r="G60" s="1">
-        <v>5.55</v>
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>5.8</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E61" s="2"/>
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" s="2">
+        <v>3</v>
+      </c>
+      <c r="F61" s="1">
+        <v>2.99</v>
+      </c>
+      <c r="G61" s="1">
+        <f>gasolina_2010[[#This Row],[PREÇO UNITARIO]]*gasolina_2010[[#This Row],[QUANTIDADE LTS]]</f>
+        <v>8.9700000000000006</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>